<commit_message>
feat: Mark diff cells and extracted diff content
</commit_message>
<xml_diff>
--- a/actuators.xlsx
+++ b/actuators.xlsx
@@ -7,61 +7,124 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ACTUATOR_IO" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
+  <si>
+    <t>序号serial number</t>
+  </si>
+  <si>
+    <t>信号位号idcode</t>
+  </si>
+  <si>
+    <t>扩展码extensioncode</t>
+  </si>
+  <si>
+    <t>信号说明designation</t>
+  </si>
+  <si>
+    <t>图号diagram number</t>
+  </si>
+  <si>
+    <t>版本rev.</t>
+  </si>
+  <si>
+    <t>备注remark</t>
+  </si>
   <si>
     <t>YTFS004VL</t>
   </si>
   <si>
+    <t>YTFS007VL</t>
+  </si>
+  <si>
     <t>YTFS060VL</t>
   </si>
   <si>
-    <t>YTFS007VL</t>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>OP</t>
   </si>
   <si>
     <t>RC</t>
   </si>
   <si>
-    <t>FP</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>OD</t>
-  </si>
-  <si>
-    <t>CD</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
   <si>
     <t>CO</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>P</t>
+    <t xml:space="preserve">关指令
+</t>
+  </si>
+  <si>
+    <t>启动给水泵出口电动阀全关
+STARTUP FWP OLET M.O.V. CLS POSN</t>
+  </si>
+  <si>
+    <t>启动给水泵出口电动阀执行机构故障
+STARTUP FWP OLET M.O.V. FLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">开指令
+</t>
+  </si>
+  <si>
+    <t>启动给水泵出口电动阀全开
+STARTUP FWP OLET M.O.V. OPEN POSN</t>
+  </si>
+  <si>
+    <t>启动给水泵出口电动阀遥控
+STARTUP FWP OLET M.O.V. REMOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>启动给水泵再循环阀全关
+STRUP FWP REIRULG VLV. CLS POSN</t>
+  </si>
+  <si>
+    <t>启动给水泵再循环阀全开
+STRUP FWP REIRULG VLV. OPEN POSN</t>
   </si>
   <si>
     <t>FD-6</t>
   </si>
   <si>
+    <t>SAMA-16</t>
+  </si>
+  <si>
     <t>FD-7</t>
   </si>
   <si>
     <t>SAMA-15</t>
   </si>
   <si>
-    <t>SAMA-16</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -419,164 +482,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>2</v>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>